<commit_message>
commit 01 - 24/07
</commit_message>
<xml_diff>
--- a/list_maker_spreadsheet.xlsx
+++ b/list_maker_spreadsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="21">
   <si>
     <t xml:space="preserve">lvl</t>
   </si>
@@ -42,6 +42,48 @@
   <si>
     <t xml:space="preserve">]</t>
   </si>
+  <si>
+    <t xml:space="preserve">Pokeball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greatball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultraball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masterball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_mount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_cave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_tunnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_safari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_valley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object_center</t>
+  </si>
 </sst>
 </file>
 
@@ -56,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,7 +158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,6 +173,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -149,25 +196,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R35" activeCellId="0" sqref="R35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="4.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="3.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="3.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="4.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="2.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="3.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="2.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="2.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="2.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="2.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -192,18 +255,34 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <f aca="false">J29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -228,11 +307,51 @@
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <f aca="false">A2 + 1</f>
         <v>2</v>
@@ -260,8 +379,51 @@
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <f aca="false">A3 + 1</f>
         <v>3</v>
@@ -289,8 +451,51 @@
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <f aca="false">A4 + 1</f>
         <v>4</v>
@@ -318,8 +523,51 @@
       <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <f aca="false">A5 + 1</f>
         <v>5</v>
@@ -347,8 +595,51 @@
       <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <f aca="false">A6 + 1</f>
         <v>6</v>
@@ -376,8 +667,51 @@
       <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <f aca="false">A7 + 1</f>
         <v>7</v>
@@ -405,8 +739,51 @@
       <c r="H8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V8" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <f aca="false">A8 + 1</f>
         <v>8</v>
@@ -434,8 +811,51 @@
       <c r="H9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V9" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <f aca="false">A9 + 1</f>
         <v>9</v>
@@ -463,8 +883,51 @@
       <c r="H10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V10" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X10" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <f aca="false">A10 + 1</f>
         <v>10</v>
@@ -492,8 +955,51 @@
       <c r="H11" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <f aca="false">A11 + 1</f>
         <v>11</v>
@@ -522,7 +1028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <f aca="false">A12 + 1</f>
         <v>12</v>
@@ -551,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <f aca="false">A13 + 1</f>
         <v>13</v>
@@ -580,7 +1086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <f aca="false">A14 + 1</f>
         <v>14</v>
@@ -609,7 +1115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <f aca="false">A15 + 1</f>
         <v>15</v>
@@ -638,7 +1144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <f aca="false">A16 + 1</f>
         <v>16</v>
@@ -667,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <f aca="false">A17 + 1</f>
         <v>17</v>
@@ -696,7 +1202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <f aca="false">A18 + 1</f>
         <v>18</v>
@@ -725,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <f aca="false">A19 + 1</f>
         <v>19</v>
@@ -754,7 +1260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <f aca="false">A20 + 1</f>
         <v>20</v>
@@ -783,7 +1289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <f aca="false">A21 + 1</f>
         <v>21</v>
@@ -812,7 +1318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <f aca="false">A22 + 1</f>
         <v>22</v>
@@ -841,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <f aca="false">A23 + 1</f>
         <v>23</v>
@@ -870,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <f aca="false">A24 + 1</f>
         <v>24</v>
@@ -899,7 +1405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <f aca="false">A25 + 1</f>
         <v>25</v>
@@ -928,7 +1434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <f aca="false">A26 + 1</f>
         <v>26</v>
@@ -957,7 +1463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <f aca="false">A27 + 1</f>
         <v>27</v>
@@ -986,7 +1492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <f aca="false">A28 + 1</f>
         <v>28</v>
@@ -1015,7 +1521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <f aca="false">A29 + 1</f>
         <v>29</v>
@@ -1044,7 +1550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <f aca="false">A30 + 1</f>
         <v>30</v>
@@ -1073,7 +1579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <f aca="false">A31 + 1</f>
         <v>31</v>
@@ -1102,7 +1608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <f aca="false">A32 + 1</f>
         <v>32</v>
@@ -1131,7 +1637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <f aca="false">A33 + 1</f>
         <v>33</v>
@@ -1160,7 +1666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <f aca="false">A34 + 1</f>
         <v>34</v>
@@ -1189,7 +1695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <f aca="false">A35 + 1</f>
         <v>35</v>
@@ -1218,7 +1724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <f aca="false">A36 + 1</f>
         <v>36</v>
@@ -1247,7 +1753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <f aca="false">A37 + 1</f>
         <v>37</v>
@@ -1276,7 +1782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <f aca="false">A38 + 1</f>
         <v>38</v>
@@ -1305,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <f aca="false">A39 + 1</f>
         <v>39</v>
@@ -1334,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <f aca="false">A40 + 1</f>
         <v>40</v>
@@ -1363,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <f aca="false">A41 + 1</f>
         <v>41</v>
@@ -1392,7 +1898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <f aca="false">A42 + 1</f>
         <v>42</v>
@@ -1421,7 +1927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <f aca="false">A43 + 1</f>
         <v>43</v>
@@ -1450,7 +1956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <f aca="false">A44 + 1</f>
         <v>44</v>
@@ -1479,7 +1985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <f aca="false">A45 + 1</f>
         <v>45</v>
@@ -1508,7 +2014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <f aca="false">A46 + 1</f>
         <v>46</v>
@@ -1537,7 +2043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <f aca="false">A47 + 1</f>
         <v>47</v>
@@ -1566,7 +2072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <f aca="false">A48 + 1</f>
         <v>48</v>
@@ -1595,7 +2101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <f aca="false">A49 + 1</f>
         <v>49</v>
@@ -1624,7 +2130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <f aca="false">A50 + 1</f>
         <v>50</v>
@@ -1653,7 +2159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <f aca="false">A51 + 1</f>
         <v>51</v>
@@ -1682,7 +2188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <f aca="false">A52 + 1</f>
         <v>52</v>
@@ -1711,7 +2217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <f aca="false">A53 + 1</f>
         <v>53</v>
@@ -1740,7 +2246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <f aca="false">A54 + 1</f>
         <v>54</v>
@@ -1769,7 +2275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <f aca="false">A55 + 1</f>
         <v>55</v>
@@ -1798,7 +2304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <f aca="false">A56 + 1</f>
         <v>56</v>
@@ -1827,7 +2333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <f aca="false">A57 + 1</f>
         <v>57</v>
@@ -1856,7 +2362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <f aca="false">A58 + 1</f>
         <v>58</v>
@@ -1885,7 +2391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <f aca="false">A59 + 1</f>
         <v>59</v>
@@ -1914,7 +2420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <f aca="false">A60 + 1</f>
         <v>60</v>
@@ -1943,7 +2449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <f aca="false">A61 + 1</f>
         <v>61</v>
@@ -1972,7 +2478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <f aca="false">A62 + 1</f>
         <v>62</v>
@@ -2001,7 +2507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <f aca="false">A63 + 1</f>
         <v>63</v>
@@ -2030,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <f aca="false">A64 + 1</f>
         <v>64</v>
@@ -2059,7 +2565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <f aca="false">A65 + 1</f>
         <v>65</v>
@@ -2088,7 +2594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <f aca="false">A66 + 1</f>
         <v>66</v>
@@ -2117,7 +2623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <f aca="false">A67 + 1</f>
         <v>67</v>
@@ -2146,7 +2652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <f aca="false">A68 + 1</f>
         <v>68</v>
@@ -2175,7 +2681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <f aca="false">A69 + 1</f>
         <v>69</v>
@@ -2204,7 +2710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <f aca="false">A70 + 1</f>
         <v>70</v>
@@ -2233,7 +2739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <f aca="false">A71 + 1</f>
         <v>71</v>
@@ -2262,7 +2768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
         <f aca="false">A72 + 1</f>
         <v>72</v>
@@ -2291,7 +2797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
         <f aca="false">A73 + 1</f>
         <v>73</v>
@@ -2320,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <f aca="false">A74 + 1</f>
         <v>74</v>
@@ -2349,7 +2855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
         <f aca="false">A75 + 1</f>
         <v>75</v>
@@ -2378,7 +2884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <f aca="false">A76 + 1</f>
         <v>76</v>
@@ -2407,7 +2913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
         <f aca="false">A77 + 1</f>
         <v>77</v>
@@ -2436,7 +2942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
         <f aca="false">A78 + 1</f>
         <v>78</v>
@@ -2465,7 +2971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
         <f aca="false">A79 + 1</f>
         <v>79</v>
@@ -2494,7 +3000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
         <f aca="false">A80 + 1</f>
         <v>80</v>
@@ -2523,7 +3029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
         <f aca="false">A81 + 1</f>
         <v>81</v>
@@ -2552,7 +3058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
         <f aca="false">A82 + 1</f>
         <v>82</v>
@@ -2581,7 +3087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
         <f aca="false">A83 + 1</f>
         <v>83</v>
@@ -2610,7 +3116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
         <f aca="false">A84 + 1</f>
         <v>84</v>
@@ -2639,7 +3145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
         <f aca="false">A85 + 1</f>
         <v>85</v>
@@ -2668,7 +3174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
         <f aca="false">A86 + 1</f>
         <v>86</v>
@@ -2697,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
         <f aca="false">A87 + 1</f>
         <v>87</v>
@@ -2726,7 +3232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
         <f aca="false">A88 + 1</f>
         <v>88</v>
@@ -2755,7 +3261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
         <f aca="false">A89 + 1</f>
         <v>89</v>
@@ -2784,7 +3290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
         <f aca="false">A90 + 1</f>
         <v>90</v>
@@ -2813,7 +3319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
         <f aca="false">A91 + 1</f>
         <v>91</v>
@@ -2842,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
         <f aca="false">A92 + 1</f>
         <v>92</v>
@@ -2871,7 +3377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
         <f aca="false">A93 + 1</f>
         <v>93</v>
@@ -2900,7 +3406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
         <f aca="false">A94 + 1</f>
         <v>94</v>
@@ -2929,7 +3435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
         <f aca="false">A95 + 1</f>
         <v>95</v>
@@ -2958,7 +3464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
         <f aca="false">A96 + 1</f>
         <v>96</v>
@@ -2987,7 +3493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
         <f aca="false">A97 + 1</f>
         <v>97</v>
@@ -3016,7 +3522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
         <f aca="false">A98 + 1</f>
         <v>98</v>
@@ -3045,7 +3551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
         <f aca="false">A99 + 1</f>
         <v>99</v>

</xml_diff>